<commit_message>
Select tab - ammend code
</commit_message>
<xml_diff>
--- a/Documentation/Lists/Other Deductions List.xlsx
+++ b/Documentation/Lists/Other Deductions List.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nahuel.delacruz\OneDrive - Sovos Compliance\Desktop\Nahuel\Projects\Returns Taxpayer documentation\Lists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/Documentation/Lists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594F85A1-C11C-46E4-9F8B-0AE332D5EF3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{594F85A1-C11C-46E4-9F8B-0AE332D5EF3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6D97546-C2F2-46D9-AA5D-44B9F6B7B3BC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{FE4AA1FC-473F-49C3-BAC8-5534CDE657C4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{FE4AA1FC-473F-49C3-BAC8-5534CDE657C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Non-Local State Forms" sheetId="1" r:id="rId1"/>
@@ -1432,7 +1432,7 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1993,7 +1993,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30C64A9E-36B7-4922-B701-6744F111C0A3}">
   <dimension ref="A1:XFA44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
@@ -8574,8 +8574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B718367-FE80-4DC9-B400-43CA3DDF32E0}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8674,7 +8674,7 @@
         <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Create Screen scraping workflow
</commit_message>
<xml_diff>
--- a/Documentation/Lists/Other Deductions List.xlsx
+++ b/Documentation/Lists/Other Deductions List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/Documentation/Lists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{594F85A1-C11C-46E4-9F8B-0AE332D5EF3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6D97546-C2F2-46D9-AA5D-44B9F6B7B3BC}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{594F85A1-C11C-46E4-9F8B-0AE332D5EF3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87DAEDF0-0249-4449-9D4D-6A9FADC83407}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{FE4AA1FC-473F-49C3-BAC8-5534CDE657C4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{FE4AA1FC-473F-49C3-BAC8-5534CDE657C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Non-Local State Forms" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,10 @@
     <sheet name="CO Locals" sheetId="2" r:id="rId3"/>
     <sheet name="LA Locals" sheetId="4" r:id="rId4"/>
     <sheet name="Bot Path" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="8" r:id="rId6"/>
+    <sheet name="Sheet4" sheetId="9" r:id="rId7"/>
+    <sheet name="ScreenScraping" sheetId="6" r:id="rId8"/>
+    <sheet name="ExportWorksheet" sheetId="7" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'LA Locals'!$A$1:$E$64</definedName>
@@ -42,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="323">
   <si>
     <t>State</t>
   </si>
@@ -980,22 +984,37 @@
     <t>Form page</t>
   </si>
   <si>
-    <t>SC ST-389</t>
-  </si>
-  <si>
-    <t>Click on text</t>
-  </si>
-  <si>
-    <t>Print Tab</t>
-  </si>
-  <si>
-    <t>Deduction</t>
-  </si>
-  <si>
-    <t>LN 4 - EDI Deductions</t>
-  </si>
-  <si>
     <t>Return Name</t>
+  </si>
+  <si>
+    <t>ReturnName</t>
+  </si>
+  <si>
+    <t>Celdas</t>
+  </si>
+  <si>
+    <t>(?&lt;=Other Legal Deductions).*</t>
+  </si>
+  <si>
+    <t>Matches</t>
+  </si>
+  <si>
+    <t>Split Regex</t>
+  </si>
+  <si>
+    <t>Expected Items</t>
+  </si>
+  <si>
+    <t>\s+</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Done. Need testing</t>
+  </si>
+  <si>
+    <t>Code Export Worksheet logic</t>
   </si>
 </sst>
 </file>
@@ -1130,6 +1149,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1432,7 +1455,7 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8572,19 +8595,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B718367-FE80-4DC9-B400-43CA3DDF32E0}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -8592,7 +8614,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="C1" t="s">
         <v>311</v>
@@ -8604,447 +8626,177 @@
         <v>306</v>
       </c>
       <c r="F1" t="s">
-        <v>308</v>
+        <v>320</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="3">
-        <v>1</v>
+        <v>37</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>314</v>
+        <v>307</v>
+      </c>
+      <c r="F2" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="3">
-        <v>2</v>
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>314</v>
+        <v>310</v>
+      </c>
+      <c r="F3" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>38</v>
+        <v>44</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2</v>
       </c>
       <c r="E4" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="3">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F685FA-063B-4F86-B13C-EA50FE5E6A1A}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8A83C5-6D54-45C5-B6DF-A13287EB41E9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D041409-A1B6-4EA0-9202-9325A1DA72A2}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C2">
         <v>2</v>
       </c>
-      <c r="E5" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="3">
-        <v>2</v>
-      </c>
-      <c r="E7" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="3">
-        <v>4</v>
-      </c>
-      <c r="E8" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" t="s">
-        <v>165</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" t="s">
-        <v>167</v>
-      </c>
-      <c r="D10" s="3">
-        <v>2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="3">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" t="s">
-        <v>171</v>
-      </c>
-      <c r="D12" s="3">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" t="s">
-        <v>174</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" t="s">
-        <v>175</v>
-      </c>
-      <c r="D16" s="3">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>57</v>
-      </c>
-      <c r="B17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" s="3">
-        <v>2</v>
-      </c>
-      <c r="E17" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" t="s">
-        <v>178</v>
-      </c>
-      <c r="D18" s="3">
-        <v>2</v>
-      </c>
-      <c r="E18" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" s="3">
-        <v>2</v>
-      </c>
-      <c r="E19" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E20" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>64</v>
-      </c>
-      <c r="B21" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>67</v>
-      </c>
-      <c r="B22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="3">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>67</v>
-      </c>
-      <c r="B23" t="s">
-        <v>69</v>
-      </c>
-      <c r="D23" s="3">
-        <v>1</v>
-      </c>
-      <c r="E23" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>70</v>
-      </c>
-      <c r="B24" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E24" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" t="s">
-        <v>73</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E25" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>74</v>
-      </c>
-      <c r="B26" t="s">
-        <v>75</v>
-      </c>
-      <c r="C26" t="s">
-        <v>75</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="D2" t="s">
+        <v>319</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81755BC5-6D66-4348-A647-E5E111A54C94}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>74</v>
-      </c>
-      <c r="B27" t="s">
-        <v>75</v>
-      </c>
-      <c r="C27" t="s">
-        <v>312</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="E27" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>77</v>
-      </c>
-      <c r="B28" t="s">
-        <v>78</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E28" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>80</v>
-      </c>
-      <c r="B29" t="s">
-        <v>81</v>
-      </c>
-      <c r="D29" s="3">
-        <v>2</v>
-      </c>
-      <c r="E29" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>82</v>
-      </c>
-      <c r="B30" t="s">
-        <v>83</v>
-      </c>
-      <c r="D30" s="3">
-        <v>4</v>
-      </c>
-      <c r="E30" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>84</v>
-      </c>
-      <c r="B31" t="s">
-        <v>85</v>
-      </c>
-      <c r="D31" s="3">
-        <v>1</v>
-      </c>
-      <c r="E31" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>86</v>
-      </c>
-      <c r="B32" t="s">
-        <v>87</v>
-      </c>
-      <c r="D32" s="3">
-        <v>2</v>
-      </c>
-      <c r="E32" t="s">
-        <v>307</v>
+      <c r="B1" t="s">
+        <v>314</v>
       </c>
     </row>
   </sheetData>

</xml_diff>